<commit_message>
aligned joey error data
</commit_message>
<xml_diff>
--- a/Test Data Per Error Type - Joey Tagged.xlsx
+++ b/Test Data Per Error Type - Joey Tagged.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2091" uniqueCount="1095">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2091" uniqueCount="1096">
   <si>
     <t>Insertion</t>
   </si>
@@ -8650,13 +8650,16 @@
   </si>
   <si>
     <t>Bahagi na ng moderno Olympic nungg una panahon ang ligsa ng sining .</t>
+  </si>
+  <si>
+    <t>puting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8981,6 +8984,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -9015,6 +9019,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -9190,14 +9195,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="70.5703125" customWidth="1"/>
     <col min="4" max="4" width="36.5703125" customWidth="1"/>
@@ -9208,7 +9213,7 @@
     <col min="9" max="9" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="63">
+    <row r="1" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -9237,7 +9242,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>480</v>
       </c>
@@ -9264,7 +9269,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>481</v>
       </c>
@@ -9291,7 +9296,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>482</v>
       </c>
@@ -9318,7 +9323,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>483</v>
       </c>
@@ -9345,7 +9350,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>484</v>
       </c>
@@ -9372,7 +9377,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45">
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>485</v>
       </c>
@@ -9399,7 +9404,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>492</v>
       </c>
@@ -9426,7 +9431,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30">
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>491</v>
       </c>
@@ -9453,7 +9458,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>495</v>
       </c>
@@ -9480,7 +9485,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>674</v>
       </c>
@@ -9507,7 +9512,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>496</v>
       </c>
@@ -9534,7 +9539,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30">
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -9555,7 +9560,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>502</v>
       </c>
@@ -9582,7 +9587,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="45">
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>503</v>
       </c>
@@ -9609,7 +9614,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30">
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -9630,7 +9635,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30">
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>48</v>
       </c>
@@ -9657,7 +9662,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>504</v>
       </c>
@@ -9684,7 +9689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30">
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>505</v>
       </c>
@@ -9711,7 +9716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="45">
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>508</v>
       </c>
@@ -9738,7 +9743,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -9759,7 +9764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30">
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>509</v>
       </c>
@@ -9786,7 +9791,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30">
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -9807,7 +9812,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="30">
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -9828,7 +9833,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30">
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>511</v>
       </c>
@@ -9855,7 +9860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30">
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>513</v>
       </c>
@@ -9882,7 +9887,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="30">
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>514</v>
       </c>
@@ -9909,7 +9914,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30">
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>515</v>
       </c>
@@ -9936,7 +9941,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30">
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>516</v>
       </c>
@@ -9963,7 +9968,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30">
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>517</v>
       </c>
@@ -9990,7 +9995,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30">
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>518</v>
       </c>
@@ -10017,7 +10022,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="45">
+    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>531</v>
       </c>
@@ -10044,7 +10049,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="45">
+    <row r="33" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>523</v>
       </c>
@@ -10071,7 +10076,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -10090,7 +10095,7 @@
       <c r="H34" s="6"/>
       <c r="I34" s="5"/>
     </row>
-    <row r="35" spans="1:14" ht="75">
+    <row r="35" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>561</v>
       </c>
@@ -10117,7 +10122,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="75">
+    <row r="36" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>561</v>
       </c>
@@ -10144,7 +10149,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="30">
+    <row r="37" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -10165,7 +10170,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="45">
+    <row r="38" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>532</v>
       </c>
@@ -10192,7 +10197,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -10211,7 +10216,7 @@
       <c r="H39" s="6"/>
       <c r="I39" s="5"/>
     </row>
-    <row r="40" spans="1:14" ht="45">
+    <row r="40" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>520</v>
       </c>
@@ -10238,7 +10243,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -10257,7 +10262,7 @@
       <c r="H41" s="6"/>
       <c r="I41" s="5"/>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -10274,7 +10279,7 @@
       <c r="H42" s="6"/>
       <c r="I42" s="5"/>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -10289,7 +10294,7 @@
       <c r="H43" s="6"/>
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>519</v>
       </c>
@@ -10316,7 +10321,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="30">
+    <row r="45" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>535</v>
       </c>
@@ -10343,7 +10348,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="30">
+    <row r="46" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>536</v>
       </c>
@@ -10375,7 +10380,7 @@
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -10399,7 +10404,7 @@
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -10417,7 +10422,7 @@
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -10441,7 +10446,7 @@
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>537</v>
       </c>
@@ -10468,7 +10473,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="30">
+    <row r="51" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>701</v>
       </c>
@@ -10495,7 +10500,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -10516,7 +10521,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="45">
+    <row r="53" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>556</v>
       </c>
@@ -10543,7 +10548,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -10562,7 +10567,7 @@
       <c r="H54" s="6"/>
       <c r="I54" s="5"/>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -10581,7 +10586,7 @@
       <c r="H55" s="6"/>
       <c r="I55" s="5"/>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>521</v>
       </c>
@@ -10608,7 +10613,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>522</v>
       </c>
@@ -10642,16 +10647,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="103.140625" customWidth="1"/>
+    <col min="2" max="3" width="70.5703125" customWidth="1"/>
     <col min="4" max="4" width="36.5703125" customWidth="1"/>
     <col min="5" max="5" width="33.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
@@ -10661,7 +10667,7 @@
     <col min="10" max="10" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="63">
+    <row r="1" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -10690,8 +10696,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>571</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -10722,8 +10728,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>572</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -10754,8 +10760,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="45">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>573</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -10784,8 +10790,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>574</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -10811,8 +10817,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
@@ -10830,8 +10836,8 @@
       <c r="H6" s="6"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="30">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
         <v>575</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -10857,8 +10863,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
         <v>576</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -10884,8 +10890,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="30">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>577</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -10911,8 +10917,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="75">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
         <v>710</v>
       </c>
       <c r="B10" s="14" t="s">
@@ -10938,8 +10944,8 @@
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="75">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
         <v>713</v>
       </c>
       <c r="B11" s="14" t="s">
@@ -10965,8 +10971,8 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="105">
-      <c r="A12" s="15" t="s">
+    <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>715</v>
       </c>
       <c r="B12" s="15" t="s">
@@ -10992,8 +10998,8 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="30">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>588</v>
       </c>
       <c r="B13" s="15" t="s">
@@ -11019,7 +11025,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>589</v>
       </c>
@@ -11046,8 +11052,8 @@
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="30">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
         <v>599</v>
       </c>
       <c r="B15" s="14" t="s">
@@ -11078,8 +11084,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="45">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
         <v>138</v>
       </c>
       <c r="B16" s="14" t="s">
@@ -11110,8 +11116,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30">
-      <c r="A17" s="14" t="s">
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
         <v>604</v>
       </c>
       <c r="B17" s="14" t="s">
@@ -11142,8 +11148,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="30">
-      <c r="A18" s="17" t="s">
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
         <v>605</v>
       </c>
       <c r="B18" s="17" t="s">
@@ -11174,8 +11180,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="45">
-      <c r="A19" s="17" t="s">
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
         <v>606</v>
       </c>
       <c r="B19" s="17" t="s">
@@ -11206,8 +11212,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="17"/>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="12" t="s">
@@ -11226,8 +11232,8 @@
       <c r="I20" s="9"/>
       <c r="J20" s="12"/>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="17"/>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="12" t="s">
@@ -11246,8 +11252,8 @@
       <c r="I21" s="9"/>
       <c r="J21" s="12"/>
     </row>
-    <row r="22" spans="1:10" ht="30">
-      <c r="A22" s="17" t="s">
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
         <v>593</v>
       </c>
       <c r="B22" s="17" t="s">
@@ -11278,8 +11284,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="1"/>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
       <c r="B23" s="31"/>
       <c r="C23" s="1"/>
       <c r="D23" s="12" t="s">
@@ -11304,8 +11310,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="45">
-      <c r="A24" s="17" t="s">
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
         <v>596</v>
       </c>
       <c r="B24" s="17" t="s">
@@ -11336,8 +11342,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="30">
-      <c r="A25" s="17" t="s">
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
         <v>597</v>
       </c>
       <c r="B25" s="17" t="s">
@@ -11368,8 +11374,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="30">
-      <c r="A26" s="17" t="s">
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
         <v>598</v>
       </c>
       <c r="B26" s="17" t="s">
@@ -11400,8 +11406,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="45">
-      <c r="A27" s="17" t="s">
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
         <v>611</v>
       </c>
       <c r="B27" s="17" t="s">
@@ -11432,8 +11438,8 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="17"/>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="12" t="s">
@@ -11452,7 +11458,7 @@
       <c r="I28" s="9"/>
       <c r="J28" s="12"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>607</v>
       </c>
@@ -11484,8 +11490,8 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="60">
-      <c r="A30" s="17" t="s">
+    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
         <v>631</v>
       </c>
       <c r="B30" s="17" t="s">
@@ -11516,8 +11522,8 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="45">
-      <c r="A31" s="17" t="s">
+    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
         <v>628</v>
       </c>
       <c r="B31" s="17" t="s">
@@ -11548,8 +11554,8 @@
         <v>207</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="1"/>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="19"/>
       <c r="B32" s="31"/>
       <c r="C32" s="1"/>
       <c r="D32" s="12" t="s">
@@ -11574,8 +11580,8 @@
         <v>207</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
-      <c r="A33" s="1"/>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="19"/>
       <c r="B33" s="31"/>
       <c r="C33" s="1"/>
       <c r="D33" s="12" t="s">
@@ -11600,8 +11606,8 @@
         <v>207</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="30">
-      <c r="A34" s="17" t="s">
+    <row r="34" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
         <v>620</v>
       </c>
       <c r="B34" s="17" t="s">
@@ -11632,8 +11638,8 @@
         <v>207</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="30">
-      <c r="A35" s="17" t="s">
+    <row r="35" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="18" t="s">
         <v>622</v>
       </c>
       <c r="B35" s="17" t="s">
@@ -11664,8 +11670,8 @@
         <v>207</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="45">
-      <c r="A36" s="17" t="s">
+    <row r="36" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
         <v>616</v>
       </c>
       <c r="B36" s="17" t="s">
@@ -11696,7 +11702,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>615</v>
       </c>
@@ -11728,8 +11734,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="30">
-      <c r="A38" s="17" t="s">
+    <row r="38" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
         <v>617</v>
       </c>
       <c r="B38" s="17" t="s">
@@ -11760,8 +11766,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="30">
-      <c r="A39" s="17" t="s">
+    <row r="39" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="18" t="s">
         <v>618</v>
       </c>
       <c r="B39" s="17" t="s">
@@ -11792,8 +11798,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="60">
-      <c r="A40" s="14" t="s">
+    <row r="40" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
         <v>619</v>
       </c>
       <c r="B40" s="14" t="s">
@@ -11822,8 +11828,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="45">
-      <c r="A41" s="14" t="s">
+    <row r="41" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="20" t="s">
         <v>632</v>
       </c>
       <c r="B41" s="14" t="s">
@@ -11852,8 +11858,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="45">
-      <c r="A42" s="14" t="s">
+    <row r="42" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="20" t="s">
         <v>635</v>
       </c>
       <c r="B42" s="14" t="s">
@@ -11882,7 +11888,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
       <c r="B43" s="32"/>
       <c r="C43" s="19"/>
@@ -11906,8 +11912,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
-      <c r="A44" s="1"/>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="19"/>
       <c r="B44" s="31"/>
       <c r="C44" s="1"/>
       <c r="D44" s="12" t="s">
@@ -11930,7 +11936,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>638</v>
       </c>
@@ -11964,8 +11970,8 @@
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
     </row>
-    <row r="46" spans="1:14" ht="60">
-      <c r="A46" s="17" t="s">
+    <row r="46" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
         <v>657</v>
       </c>
       <c r="B46" s="17" t="s">
@@ -11996,8 +12002,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="60">
-      <c r="A47" s="9" t="s">
+    <row r="47" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>658</v>
       </c>
       <c r="B47" s="9" t="s">
@@ -12028,8 +12034,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
-      <c r="A48" t="s">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>637</v>
       </c>
       <c r="B48" t="s">
@@ -12060,8 +12066,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="45">
-      <c r="A49" s="13" t="s">
+    <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
         <v>654</v>
       </c>
       <c r="B49" s="13" t="s">
@@ -12092,8 +12098,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="45">
-      <c r="A50" s="21" t="s">
+    <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
         <v>645</v>
       </c>
       <c r="B50" s="21" t="s">
@@ -12124,8 +12130,8 @@
         <v>211</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
-      <c r="A51" s="21" t="s">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
         <v>641</v>
       </c>
       <c r="B51" s="21" t="s">
@@ -12156,8 +12162,8 @@
         <v>211</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="30">
-      <c r="A52" s="21" t="s">
+    <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="22" t="s">
         <v>646</v>
       </c>
       <c r="B52" s="21" t="s">
@@ -12188,8 +12194,8 @@
         <v>218</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="45">
-      <c r="A53" s="9" t="s">
+    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>648</v>
       </c>
       <c r="B53" s="9" t="s">
@@ -12220,8 +12226,8 @@
         <v>221</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="60">
-      <c r="A54" s="21" t="s">
+    <row r="54" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="s">
         <v>750</v>
       </c>
       <c r="B54" s="21" t="s">
@@ -12252,8 +12258,8 @@
         <v>221</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
-      <c r="A55" s="11" t="s">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
         <v>224</v>
       </c>
       <c r="B55" s="11" t="s">
@@ -12284,8 +12290,8 @@
         <v>227</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="30">
-      <c r="A56" s="9" t="s">
+    <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>644</v>
       </c>
       <c r="B56" s="9" t="s">
@@ -12313,8 +12319,8 @@
         <v>230</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="60">
-      <c r="A57" s="9" t="s">
+    <row r="57" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>667</v>
       </c>
       <c r="B57" s="9" t="s">
@@ -12345,8 +12351,8 @@
         <v>230</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="45">
-      <c r="A58" s="9" t="s">
+    <row r="58" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
         <v>652</v>
       </c>
       <c r="B58" s="9" t="s">
@@ -12377,8 +12383,8 @@
         <v>235</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="45">
-      <c r="A59" s="9" t="s">
+    <row r="59" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
         <v>666</v>
       </c>
       <c r="B59" s="9" t="s">
@@ -12409,8 +12415,8 @@
         <v>238</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="30">
-      <c r="A60" s="9" t="s">
+    <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
         <v>660</v>
       </c>
       <c r="B60" s="9" t="s">
@@ -12441,7 +12447,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
         <v>663</v>
       </c>
@@ -12471,14 +12477,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="70.5703125" customWidth="1"/>
     <col min="4" max="4" width="36.5703125" customWidth="1"/>
@@ -12489,7 +12495,7 @@
     <col min="9" max="9" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="63">
+    <row r="1" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -12518,7 +12524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>760</v>
       </c>
@@ -12547,7 +12553,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>798</v>
       </c>
@@ -12576,7 +12582,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D4" s="24" t="s">
         <v>247</v>
       </c>
@@ -12596,7 +12602,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" s="24" t="s">
         <v>44</v>
       </c>
@@ -12616,7 +12622,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="45">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
         <v>802</v>
       </c>
@@ -12645,7 +12651,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="45">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>808</v>
       </c>
@@ -12674,7 +12680,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="24" t="s">
         <v>251</v>
       </c>
@@ -12694,7 +12700,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="45">
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>805</v>
       </c>
@@ -12723,7 +12729,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
         <v>806</v>
       </c>
@@ -12752,7 +12758,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="45">
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>807</v>
       </c>
@@ -12781,7 +12787,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="60">
+    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
         <v>811</v>
       </c>
@@ -12810,7 +12816,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="60">
+    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
         <v>1016</v>
       </c>
@@ -12839,7 +12845,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="36"/>
       <c r="C14" s="24"/>
@@ -12862,7 +12868,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="45">
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>263</v>
       </c>
@@ -12894,7 +12900,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="75">
+    <row r="16" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
         <v>814</v>
       </c>
@@ -12926,7 +12932,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="45">
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
         <v>819</v>
       </c>
@@ -12958,7 +12964,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="45">
+    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
         <v>824</v>
       </c>
@@ -12990,7 +12996,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="45">
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
         <v>820</v>
       </c>
@@ -13022,7 +13028,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="60">
+    <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="36" t="s">
         <v>821</v>
       </c>
@@ -13054,7 +13060,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="30">
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="D21" s="24" t="s">
         <v>275</v>
       </c>
@@ -13077,7 +13083,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D22" s="36" t="s">
         <v>826</v>
       </c>
@@ -13098,7 +13104,7 @@
       </c>
       <c r="J22" s="24"/>
     </row>
-    <row r="23" spans="1:10" ht="75">
+    <row r="23" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
         <v>846</v>
       </c>
@@ -13130,7 +13136,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="60">
+    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>851</v>
       </c>
@@ -13162,7 +13168,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="30">
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="36"/>
       <c r="B25" s="36"/>
       <c r="C25" s="36"/>
@@ -13182,7 +13188,7 @@
       <c r="I25" s="23"/>
       <c r="J25" s="24"/>
     </row>
-    <row r="26" spans="1:10" ht="45">
+    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="36" t="s">
         <v>844</v>
       </c>
@@ -13214,7 +13220,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="30">
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="36" t="s">
         <v>845</v>
       </c>
@@ -13246,7 +13252,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="30">
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
         <v>829</v>
       </c>
@@ -13278,7 +13284,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="30">
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="s">
         <v>830</v>
       </c>
@@ -13310,7 +13316,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="30">
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="36" t="s">
         <v>835</v>
       </c>
@@ -13342,7 +13348,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="60">
+    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
         <v>1032</v>
       </c>
@@ -13374,7 +13380,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="30">
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="36" t="s">
         <v>834</v>
       </c>
@@ -13406,7 +13412,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="45">
+    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="36" t="s">
         <v>1036</v>
       </c>
@@ -13438,7 +13444,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="45">
+    <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="36" t="s">
         <v>838</v>
       </c>
@@ -13470,7 +13476,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="45">
+    <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
         <v>301</v>
       </c>
@@ -13502,7 +13508,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="45">
+    <row r="36" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
         <v>842</v>
       </c>
@@ -13534,7 +13540,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="60">
+    <row r="37" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="36" t="s">
         <v>860</v>
       </c>
@@ -13566,7 +13572,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="36"/>
       <c r="B38" s="36"/>
       <c r="C38" s="36"/>
@@ -13590,7 +13596,7 @@
       </c>
       <c r="J38" s="24"/>
     </row>
-    <row r="39" spans="1:10" ht="30">
+    <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="36" t="s">
         <v>843</v>
       </c>
@@ -13622,7 +13628,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="45">
+    <row r="40" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="36" t="s">
         <v>865</v>
       </c>
@@ -13654,7 +13660,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="75">
+    <row r="41" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="36" t="s">
         <v>855</v>
       </c>
@@ -13686,7 +13692,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="36"/>
       <c r="B42" s="36"/>
       <c r="C42" s="36"/>
@@ -13710,7 +13716,7 @@
       </c>
       <c r="J42" s="24"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="36"/>
       <c r="B43" s="36"/>
       <c r="C43" s="36"/>
@@ -13734,7 +13740,7 @@
       </c>
       <c r="J43" s="24"/>
     </row>
-    <row r="44" spans="1:10" ht="45">
+    <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="36" t="s">
         <v>856</v>
       </c>
@@ -13766,7 +13772,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="36"/>
       <c r="B45" s="36"/>
       <c r="C45" s="36"/>
@@ -13790,7 +13796,7 @@
       </c>
       <c r="J45" s="24"/>
     </row>
-    <row r="46" spans="1:10" ht="45">
+    <row r="46" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="36" t="s">
         <v>857</v>
       </c>
@@ -13822,7 +13828,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="36"/>
       <c r="B47" s="36"/>
       <c r="C47" s="36"/>
@@ -13846,7 +13852,7 @@
       </c>
       <c r="J47" s="24"/>
     </row>
-    <row r="48" spans="1:10" ht="60">
+    <row r="48" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="36" t="s">
         <v>888</v>
       </c>
@@ -13878,7 +13884,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="30">
+    <row r="49" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="36" t="s">
         <v>886</v>
       </c>
@@ -13914,7 +13920,7 @@
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
     </row>
-    <row r="50" spans="1:14" ht="45">
+    <row r="50" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="36" t="s">
         <v>887</v>
       </c>
@@ -13946,7 +13952,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="75">
+    <row r="51" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="36" t="s">
         <v>889</v>
       </c>
@@ -13978,7 +13984,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="36"/>
       <c r="B52" s="36"/>
       <c r="C52" s="36"/>
@@ -14002,7 +14008,7 @@
       </c>
       <c r="J52" s="24"/>
     </row>
-    <row r="53" spans="1:14" ht="45">
+    <row r="53" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="36" t="s">
         <v>890</v>
       </c>
@@ -14034,7 +14040,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="30">
+    <row r="54" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="38"/>
       <c r="C54" s="38"/>
       <c r="D54" s="24" t="s">
@@ -14059,7 +14065,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="30">
+    <row r="55" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="36" t="s">
         <v>878</v>
       </c>
@@ -14091,7 +14097,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="60">
+    <row r="56" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="36" t="s">
         <v>879</v>
       </c>
@@ -14123,7 +14129,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="45">
+    <row r="57" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="36" t="s">
         <v>880</v>
       </c>
@@ -14155,7 +14161,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="45">
+    <row r="58" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="36" t="s">
         <v>881</v>
       </c>
@@ -14187,7 +14193,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="45">
+    <row r="59" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="24"/>
       <c r="B59" s="24"/>
       <c r="C59" s="24"/>
@@ -14213,7 +14219,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="45">
+    <row r="60" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="24"/>
       <c r="B60" s="24"/>
       <c r="C60" s="24"/>
@@ -14239,7 +14245,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="45">
+    <row r="61" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="36" t="s">
         <v>898</v>
       </c>
@@ -14271,7 +14277,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="30">
+    <row r="62" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="36" t="s">
         <v>919</v>
       </c>
@@ -14303,7 +14309,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="30">
+    <row r="63" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="36" t="s">
         <v>899</v>
       </c>
@@ -14335,7 +14341,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="45">
+    <row r="64" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="36" t="s">
         <v>900</v>
       </c>
@@ -14367,7 +14373,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="75">
+    <row r="65" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="36" t="s">
         <v>925</v>
       </c>
@@ -14399,7 +14405,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="45">
+    <row r="66" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="36" t="s">
         <v>901</v>
       </c>
@@ -14431,7 +14437,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="45">
+    <row r="67" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="36" t="s">
         <v>902</v>
       </c>
@@ -14463,7 +14469,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="45">
+    <row r="68" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="36" t="s">
         <v>904</v>
       </c>
@@ -14495,7 +14501,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="45">
+    <row r="69" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="36" t="s">
         <v>927</v>
       </c>
@@ -14527,7 +14533,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="60">
+    <row r="70" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="36" t="s">
         <v>928</v>
       </c>
@@ -14559,7 +14565,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="105">
+    <row r="71" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A71" s="36" t="s">
         <v>930</v>
       </c>
@@ -14591,7 +14597,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="45">
+    <row r="72" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="36" t="s">
         <v>906</v>
       </c>
@@ -14623,7 +14629,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="45">
+    <row r="73" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="36" t="s">
         <v>907</v>
       </c>
@@ -14655,7 +14661,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="45">
+    <row r="74" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="36" t="s">
         <v>909</v>
       </c>
@@ -14687,7 +14693,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="45">
+    <row r="75" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="D75" s="24" t="s">
         <v>380</v>
       </c>
@@ -14710,7 +14716,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="45">
+    <row r="76" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="36" t="s">
         <v>915</v>
       </c>
@@ -14742,7 +14748,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="45">
+    <row r="77" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="24"/>
       <c r="B77" s="24"/>
       <c r="C77" s="24"/>
@@ -14768,7 +14774,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="24"/>
       <c r="B78" s="24"/>
       <c r="C78" s="24"/>
@@ -14792,7 +14798,7 @@
       </c>
       <c r="J78" s="24"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="24"/>
       <c r="B79" s="24"/>
       <c r="C79" s="24"/>
@@ -14816,7 +14822,7 @@
       </c>
       <c r="J79" s="24"/>
     </row>
-    <row r="80" spans="1:10" ht="45">
+    <row r="80" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="36" t="s">
         <v>933</v>
       </c>
@@ -14848,7 +14854,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="45">
+    <row r="81" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="36" t="s">
         <v>932</v>
       </c>
@@ -14880,7 +14886,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="45">
+    <row r="82" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="36" t="s">
         <v>958</v>
       </c>
@@ -14912,7 +14918,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="30">
+    <row r="83" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="36" t="s">
         <v>934</v>
       </c>
@@ -14944,7 +14950,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="30">
+    <row r="84" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="36" t="s">
         <v>956</v>
       </c>
@@ -14976,7 +14982,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="30">
+    <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="36" t="s">
         <v>940</v>
       </c>
@@ -15008,7 +15014,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="30">
+    <row r="86" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="36" t="s">
         <v>936</v>
       </c>
@@ -15040,7 +15046,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="30">
+    <row r="87" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="36" t="s">
         <v>935</v>
       </c>
@@ -15072,7 +15078,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="45">
+    <row r="88" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="36" t="s">
         <v>944</v>
       </c>
@@ -15104,7 +15110,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="30">
+    <row r="89" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="36" t="s">
         <v>941</v>
       </c>
@@ -15136,7 +15142,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="30">
+    <row r="90" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="24"/>
       <c r="B90" s="24"/>
       <c r="C90" s="24"/>
@@ -15162,7 +15168,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="45">
+    <row r="91" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="36" t="s">
         <v>970</v>
       </c>
@@ -15194,7 +15200,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="36"/>
       <c r="B92" s="36"/>
       <c r="C92" s="36"/>
@@ -15218,7 +15224,7 @@
       </c>
       <c r="J92" s="24"/>
     </row>
-    <row r="93" spans="1:10" ht="30">
+    <row r="93" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="36" t="s">
         <v>946</v>
       </c>
@@ -15250,7 +15256,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="24"/>
       <c r="B94" s="36"/>
       <c r="C94" s="24"/>
@@ -15274,7 +15280,7 @@
       </c>
       <c r="J94" s="24"/>
     </row>
-    <row r="95" spans="1:10" ht="30">
+    <row r="95" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="36" t="s">
         <v>950</v>
       </c>
@@ -15306,7 +15312,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="30">
+    <row r="96" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="36" t="s">
         <v>953</v>
       </c>
@@ -15338,7 +15344,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="45">
+    <row r="97" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="36" t="s">
         <v>961</v>
       </c>
@@ -15370,7 +15376,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="45">
+    <row r="98" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="36" t="s">
         <v>966</v>
       </c>
@@ -15402,7 +15408,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="45">
+    <row r="99" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="36" t="s">
         <v>971</v>
       </c>
@@ -15434,7 +15440,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="45">
+    <row r="100" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="36" t="s">
         <v>965</v>
       </c>
@@ -15466,7 +15472,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="30">
+    <row r="101" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="36" t="s">
         <v>964</v>
       </c>
@@ -15498,7 +15504,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="30">
+    <row r="102" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="36" t="s">
         <v>963</v>
       </c>
@@ -15530,7 +15536,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="30">
+    <row r="103" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="36" t="s">
         <v>962</v>
       </c>
@@ -15562,7 +15568,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="60">
+    <row r="104" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A104" s="36" t="s">
         <v>969</v>
       </c>
@@ -15594,7 +15600,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="60">
+    <row r="105" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" s="36" t="s">
         <v>979</v>
       </c>
@@ -15626,7 +15632,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="75">
+    <row r="106" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A106" s="36" t="s">
         <v>978</v>
       </c>
@@ -15658,7 +15664,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="60">
+    <row r="107" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A107" s="36" t="s">
         <v>980</v>
       </c>
@@ -15690,7 +15696,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="36"/>
       <c r="B108" s="36"/>
       <c r="C108" s="36"/>
@@ -15714,7 +15720,7 @@
       </c>
       <c r="J108" s="24"/>
     </row>
-    <row r="109" spans="1:10" ht="60">
+    <row r="109" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A109" s="36" t="s">
         <v>981</v>
       </c>
@@ -15746,7 +15752,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="60">
+    <row r="110" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A110" s="36" t="s">
         <v>982</v>
       </c>
@@ -15785,14 +15791,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="59.85546875" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
@@ -15804,7 +15810,7 @@
     <col min="10" max="10" width="40.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="42">
+    <row r="1" spans="1:10" ht="42" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -15833,7 +15839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="75">
+    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>993</v>
       </c>
@@ -15860,7 +15866,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="90">
+    <row r="3" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>995</v>
       </c>
@@ -15887,7 +15893,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="90">
+    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>713</v>
       </c>
@@ -15914,7 +15920,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>762</v>
       </c>
@@ -15941,7 +15947,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="63">
+    <row r="6" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>763</v>
       </c>
@@ -15971,7 +15977,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="63">
+    <row r="7" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>764</v>
       </c>
@@ -16001,7 +16007,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="63">
+    <row r="8" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>1001</v>
       </c>
@@ -16031,7 +16037,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="47.25">
+    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>765</v>
       </c>
@@ -16061,7 +16067,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75">
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
@@ -16069,7 +16075,7 @@
         <v>779</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>779</v>
+        <v>1095</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>28</v>
@@ -16081,7 +16087,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="35"/>
     </row>
-    <row r="11" spans="1:10" ht="47.25">
+    <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>780</v>
       </c>
@@ -16111,7 +16117,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75">
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="34"/>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
@@ -16131,7 +16137,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="35"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75">
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="34"/>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
@@ -16151,7 +16157,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="35"/>
     </row>
-    <row r="14" spans="1:10" ht="31.5">
+    <row r="14" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
         <v>766</v>
       </c>
@@ -16181,7 +16187,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="31.5">
+    <row r="15" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>767</v>
       </c>
@@ -16211,7 +16217,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="47.25">
+    <row r="16" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
         <v>768</v>
       </c>
@@ -16241,7 +16247,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="94.5">
+    <row r="17" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
         <v>796</v>
       </c>
@@ -16271,7 +16277,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="47.25">
+    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
         <v>769</v>
       </c>
@@ -16301,7 +16307,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="47.25">
+    <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
         <v>770</v>
       </c>
@@ -16331,7 +16337,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="78.75">
+    <row r="20" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
         <v>795</v>
       </c>
@@ -16361,7 +16367,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -16372,7 +16378,7 @@
       <c r="H21" s="6"/>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -16383,7 +16389,7 @@
       <c r="H22" s="6"/>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -16394,7 +16400,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -16405,7 +16411,7 @@
       <c r="H24" s="6"/>
       <c r="I24" s="5"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -16416,7 +16422,7 @@
       <c r="H25" s="6"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -16427,7 +16433,7 @@
       <c r="H26" s="6"/>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -16438,7 +16444,7 @@
       <c r="H27" s="6"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -16449,7 +16455,7 @@
       <c r="H28" s="6"/>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -16460,7 +16466,7 @@
       <c r="H29" s="6"/>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -16471,7 +16477,7 @@
       <c r="H30" s="6"/>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -16482,7 +16488,7 @@
       <c r="H31" s="6"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -16493,7 +16499,7 @@
       <c r="H32" s="6"/>
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -16504,7 +16510,7 @@
       <c r="H33" s="6"/>
       <c r="I33" s="5"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -16515,7 +16521,7 @@
       <c r="H34" s="6"/>
       <c r="I34" s="5"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -16526,7 +16532,7 @@
       <c r="H35" s="6"/>
       <c r="I35" s="5"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -16537,7 +16543,7 @@
       <c r="H36" s="6"/>
       <c r="I36" s="5"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -16548,7 +16554,7 @@
       <c r="H37" s="6"/>
       <c r="I37" s="5"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -16559,7 +16565,7 @@
       <c r="H38" s="6"/>
       <c r="I38" s="5"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -16570,7 +16576,7 @@
       <c r="H39" s="6"/>
       <c r="I39" s="5"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -16581,7 +16587,7 @@
       <c r="H40" s="6"/>
       <c r="I40" s="5"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -16592,7 +16598,7 @@
       <c r="H41" s="6"/>
       <c r="I41" s="5"/>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -16603,7 +16609,7 @@
       <c r="H42" s="6"/>
       <c r="I42" s="5"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -16614,7 +16620,7 @@
       <c r="H43" s="6"/>
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -16625,7 +16631,7 @@
       <c r="H44" s="6"/>
       <c r="I44" s="5"/>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -16636,7 +16642,7 @@
       <c r="H45" s="6"/>
       <c r="I45" s="5"/>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -16647,7 +16653,7 @@
       <c r="H46" s="6"/>
       <c r="I46" s="5"/>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -16658,7 +16664,7 @@
       <c r="H47" s="6"/>
       <c r="I47" s="5"/>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -16669,7 +16675,7 @@
       <c r="H48" s="6"/>
       <c r="I48" s="5"/>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -16680,7 +16686,7 @@
       <c r="H49" s="6"/>
       <c r="I49" s="5"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>

</xml_diff>